<commit_message>
[ MOSIP-20747 ] updated identity_schema.xlsx
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Mosip Sample identity</t>
   </si>
   <si>
-    <t xml:space="preserve">{"id":"1001","idVersion":0.1,"schemaJson":"{\"$schema\":\"http:\\/\\/json-schema.org\\/draft-07\\/schema#\",\"description\":\"MOSIP Sample identity\",\"additionalProperties\":false,\"title\":\"MOSIP identity\",\"type\":\"object\",\"definitions\":{\"simpleType\":{\"uniqueItems\":true,\"additionalItems\":false,\"type\":\"array\",\"items\":{\"additionalProperties\":false,\"type\":\"object\",\"required\":[\"language\",\"value\"],\"properties\":{\"language\":{\"type\":\"string\"},\"value\":{\"type\":\"string\"}}}},\"documentType\":{\"additionalProperties\":false,\"type\":\"object\",\"properties\":{\"format\":{\"type\":\"string\"},\"type\":{\"type\":\"string\"},\"value\":{\"type\":\"string\"},\"refNumber\":{\"type\":[\"string\",\"null\"]}}},\"biometricsType\":{\"additionalProperties\":false,\"type\":\"object\",\"properties\":{\"format\":{\"type\":\"string\"},\"version\":{\"type\":\"number\",\"minimum\":0},\"value\":{\"type\":\"string\"}}}},\"properties\":{\"identity\":{\"additionalProperties\":false,\"type\":\"object\",\"required\":[\"IDSchemaVersion\",\"fullName\",\"dateOfBirth\",\"gender\",\"addressLine1\",\"addressLine2\",\"addressLine3\",\"region\",\"province\",\"city\",\"zone\",\"postalCode\",\"phone\",\"email\",\"proofOfIdentity\",\"individualBiometrics\"],\"properties\":{\"proofOfAddress\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"gender\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"city\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"postalCode\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[(?i)A-Z0-9]{5}$|^NA$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"proofOfException-1\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"referenceIdentityNumber\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^([0-9]{10,30})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"kyc\",\"type\":\"string\",\"fieldType\":\"default\"},\"individualBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"province\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"zone\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"proofOfDateOfBirth\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"addressLine1\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"addressLine2\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"residenceStatus\":{\"bioAttributes\":[],\"fieldCategory\":\"kyc\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"addressLine3\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"email\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[A-Za-z0-9_\\\\-]+(\\\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\\\.[A-Za-z0-9_]+)*(\\\\.[a-zA-Z]{2,})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerRID\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"fullName\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"dateOfBirth\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])\\/([0][1-9]|1[0-2])\\/([0][1-9]|[1-2][0-9]|3[01])$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"individualAuthBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"introducerUIN\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"proofOfIdentity\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"IDSchemaVersion\":{\"bioAttributes\":[],\"fieldCategory\":\"none\",\"format\":\"none\",\"type\":\"number\",\"fieldType\":\"default\",\"minimum\":0},\"proofOfException\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"phone\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[+]*([0-9]{1})([0-9]{9})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerName\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"proofOfRelationship\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"UIN\":{\"bioAttributes\":[],\"fieldCategory\":\"none\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"region\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"}}}}}","effectiveFrom":"2022-03-15T06:05:25.152","settings":[{"name":"scheduledjobs","description":{"ara":"إعدادات الوظائف المجدولة","fra":"Paramètres des travaux planifiés","eng":"Scheduled Jobs Settings"},"label":{"ara":"إعدادات الوظائف المجدولة","fra":"Paramètres des travaux planifiés","eng":"Scheduled Jobs Settings"},"fxml":"ScheduledJobsSettings.fxml","icon":"scheduledjobs.png","order":"1","shortcut-icon":"scheduledjobs-shortcut.png","access-control":["REGISTRATION_SUPERVISOR"]},{"name":"globalconfigs","description":{"ara":"إعدادات التكوين العامة","fra":"Paramètres de configuration globale","eng":"Global Config Settings"},"label":{"ara":"إعدادات التكوين العامة","fra":"Paramètres de configuration globale","eng":"Global Config Settings"},"fxml":"GlobalConfigSettings.fxml","icon":"globalconfigs.png","order":"2","shortcut-icon":"globalconfigs-shortcut.png","access-control":["REGISTRATION_SUPERVISOR","REGISTRATION_OFFICER"]},{"name":"devices","description":{"ara":"إعدادات الجهاز","fra":"Réglages de l'appareil","eng":"Device Settings"},"label":{"ara":"إعدادات الجهاز","fra":"Réglages de l'appareil","eng":"Device Settings"},"fxml":"DeviceSettings.fxml","icon":"devices.png","order":"3","shortcut-icon":"devices-shortcut.png","access-control":["REGISTRATION_SUPERVISOR","REGISTRATION_OFFICER"]}]}</t>
+    <t xml:space="preserve">{\"$schema\":\"http:\\/\\/json-schema.org\\/draft-07\\/schema#\",\"description\":\"MOSIP Sample identity\",\"additionalProperties\":false,\"title\":\"MOSIP identity\",\"type\":\"object\",\"definitions\":{\"simpleType\":{\"uniqueItems\":true,\"additionalItems\":false,\"type\":\"array\",\"items\":{\"additionalProperties\":false,\"type\":\"object\",\"required\":[\"language\",\"value\"],\"properties\":{\"language\":{\"type\":\"string\"},\"value\":{\"type\":\"string\"}}}},\"documentType\":{\"additionalProperties\":false,\"type\":\"object\",\"properties\":{\"format\":{\"type\":\"string\"},\"type\":{\"type\":\"string\"},\"value\":{\"type\":\"string\"},\"refNumber\":{\"type\":[\"string\",\"null\"]}}},\"biometricsType\":{\"additionalProperties\":false,\"type\":\"object\",\"properties\":{\"format\":{\"type\":\"string\"},\"version\":{\"type\":\"number\",\"minimum\":0},\"value\":{\"type\":\"string\"}}}},\"properties\":{\"identity\":{\"additionalProperties\":false,\"type\":\"object\",\"required\":[\"IDSchemaVersion\",\"fullName\",\"dateOfBirth\",\"gender\",\"addressLine1\",\"addressLine2\",\"addressLine3\",\"region\",\"province\",\"city\",\"zone\",\"postalCode\",\"phone\",\"email\",\"proofOfIdentity\",\"individualBiometrics\"],\"properties\":{\"proofOfAddress\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"gender\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"city\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"postalCode\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[(?i)A-Z0-9]{5}$|^NA$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"proofOfException-1\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"referenceIdentityNumber\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^([0-9]{10,30})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"kyc\",\"type\":\"string\",\"fieldType\":\"default\"},\"individualBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"province\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"zone\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"proofOfDateOfBirth\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"addressLine1\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"addressLine2\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"residenceStatus\":{\"bioAttributes\":[],\"fieldCategory\":\"kyc\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"addressLine3\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"email\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[A-Za-z0-9_\\\\-]+(\\\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\\\.[A-Za-z0-9_]+)*(\\\\.[a-zA-Z]{2,})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerRID\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"fullName\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"dateOfBirth\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])\\/([0][1-9]|1[0-2])\\/([0][1-9]|[1-2][0-9]|3[01])$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"individualAuthBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"introducerUIN\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"proofOfIdentity\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"IDSchemaVersion\":{\"bioAttributes\":[],\"fieldCategory\":\"none\",\"format\":\"none\",\"type\":\"number\",\"fieldType\":\"default\",\"minimum\":0},\"proofOfException\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"phone\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[+]*([0-9]{1})([0-9]{9})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerName\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"proofOfRelationship\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"UIN\":{\"bioAttributes\":[],\"fieldCategory\":\"none\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"region\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"}}}}}</t>
   </si>
   <si>
     <t xml:space="preserve">PUBLISHED</t>
@@ -208,8 +208,8 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[ MOSIP-20747 ] fixed json in identity_schema.xlsx
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Mosip Sample identity</t>
   </si>
   <si>
-    <t xml:space="preserve">{\"$schema\":\"http:\\/\\/json-schema.org\\/draft-07\\/schema#\",\"description\":\"MOSIP Sample identity\",\"additionalProperties\":false,\"title\":\"MOSIP identity\",\"type\":\"object\",\"definitions\":{\"simpleType\":{\"uniqueItems\":true,\"additionalItems\":false,\"type\":\"array\",\"items\":{\"additionalProperties\":false,\"type\":\"object\",\"required\":[\"language\",\"value\"],\"properties\":{\"language\":{\"type\":\"string\"},\"value\":{\"type\":\"string\"}}}},\"documentType\":{\"additionalProperties\":false,\"type\":\"object\",\"properties\":{\"format\":{\"type\":\"string\"},\"type\":{\"type\":\"string\"},\"value\":{\"type\":\"string\"},\"refNumber\":{\"type\":[\"string\",\"null\"]}}},\"biometricsType\":{\"additionalProperties\":false,\"type\":\"object\",\"properties\":{\"format\":{\"type\":\"string\"},\"version\":{\"type\":\"number\",\"minimum\":0},\"value\":{\"type\":\"string\"}}}},\"properties\":{\"identity\":{\"additionalProperties\":false,\"type\":\"object\",\"required\":[\"IDSchemaVersion\",\"fullName\",\"dateOfBirth\",\"gender\",\"addressLine1\",\"addressLine2\",\"addressLine3\",\"region\",\"province\",\"city\",\"zone\",\"postalCode\",\"phone\",\"email\",\"proofOfIdentity\",\"individualBiometrics\"],\"properties\":{\"proofOfAddress\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"gender\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"city\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"postalCode\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[(?i)A-Z0-9]{5}$|^NA$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"proofOfException-1\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"referenceIdentityNumber\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^([0-9]{10,30})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"kyc\",\"type\":\"string\",\"fieldType\":\"default\"},\"individualBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"province\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"zone\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"proofOfDateOfBirth\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"addressLine1\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"addressLine2\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"residenceStatus\":{\"bioAttributes\":[],\"fieldCategory\":\"kyc\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"addressLine3\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"email\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[A-Za-z0-9_\\\\-]+(\\\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\\\.[A-Za-z0-9_]+)*(\\\\.[a-zA-Z]{2,})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerRID\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"fullName\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{3,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"dateOfBirth\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])\\/([0][1-9]|1[0-2])\\/([0][1-9]|[1-2][0-9]|3[01])$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"individualAuthBiometrics\":{\"bioAttributes\":[\"leftEye\",\"rightEye\",\"rightIndex\",\"rightLittle\",\"rightRing\",\"rightMiddle\",\"leftIndex\",\"leftLittle\",\"leftRing\",\"leftMiddle\",\"leftThumb\",\"rightThumb\",\"face\"],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/biometricsType\"},\"introducerUIN\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"proofOfIdentity\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"IDSchemaVersion\":{\"bioAttributes\":[],\"fieldCategory\":\"none\",\"format\":\"none\",\"type\":\"number\",\"fieldType\":\"default\",\"minimum\":0},\"proofOfException\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"phone\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^[+]*([0-9]{1})([0-9]{9})$\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"introducerName\":{\"bioAttributes\":[],\"fieldCategory\":\"evidence\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"},\"proofOfRelationship\":{\"bioAttributes\":[],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/documentType\"},\"UIN\":{\"bioAttributes\":[],\"fieldCategory\":\"none\",\"format\":\"none\",\"type\":\"string\",\"fieldType\":\"default\"},\"region\":{\"bioAttributes\":[],\"validators\":[{\"validator\":\"^(?=.{0,50}$).*\",\"arguments\":[],\"type\":\"regex\"}],\"fieldCategory\":\"pvt\",\"format\":\"none\",\"fieldType\":\"default\",\"$ref\":\"#\\/definitions\\/simpleType\"}}}}}</t>
+    <t xml:space="preserve">{"$schema":"http:\/\/json-schema.org\/draft-07\/schema#","description":"MOSIP Sample identity","additionalProperties":false,"title":"MOSIP identity","type":"object","definitions":{"simpleType":{"uniqueItems":true,"additionalItems":false,"type":"array","items":{"additionalProperties":false,"type":"object","required":["language","value"],"properties":{"language":{"type":"string"},"value":{"type":"string"}}}},"documentType":{"additionalProperties":false,"type":"object","properties":{"format":{"type":"string"},"type":{"type":"string"},"value":{"type":"string"},"refNumber":{"type":["string","null"]}}},"biometricsType":{"additionalProperties":false,"type":"object","properties":{"format":{"type":"string"},"version":{"type":"number","minimum":0},"value":{"type":"string"}}}},"properties":{"identity":{"additionalProperties":false,"type":"object","required":["IDSchemaVersion","fullName","dateOfBirth","gender","addressLine1","addressLine2","addressLine3","region","province","city","zone","postalCode","phone","email","proofOfIdentity","individualBiometrics"],"properties":{"proofOfAddress":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"gender":{"bioAttributes":[],"fieldCategory":"pvt","format":"","fieldType":"default","$ref":"#\/definitions\/simpleType"},"city":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"postalCode":{"bioAttributes":[],"validators":[{"validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"proofOfException-1":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"referenceIdentityNumber":{"bioAttributes":[],"validators":[{"validator":"^([0-9]{10,30})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"kyc","type":"string","fieldType":"default"},"individualBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/biometricsType"},"province":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"zone":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"proofOfDateOfBirth":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"addressLine1":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"addressLine2":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"residenceStatus":{"bioAttributes":[],"fieldCategory":"kyc","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"addressLine3":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"email":{"bioAttributes":[],"validators":[{"validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"introducerRID":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"introducerBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/biometricsType"},"fullName":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"dateOfBirth":{"bioAttributes":[],"validators":[{"validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])\/([0][1-9]|1[0-2])\/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"individualAuthBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/biometricsType"},"introducerUIN":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"proofOfIdentity":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"IDSchemaVersion":{"bioAttributes":[],"fieldCategory":"none","format":"none","type":"number","fieldType":"default","minimum":0},"proofOfException":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"phone":{"bioAttributes":[],"validators":[{"validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"introducerName":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"proofOfRelationship":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"UIN":{"bioAttributes":[],"fieldCategory":"none","format":"none","type":"string","fieldType":"default"},"region":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"}}}}}</t>
   </si>
   <si>
     <t xml:space="preserve">PUBLISHED</t>
@@ -208,8 +208,8 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
changes related to resident type documents
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroTech\IdeaProjects\mosip-data-mec\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8963A37E-93E4-491C-9DFF-F97E80FE6C01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED95FAFC-2F6C-4A30-B3C4-2150409916D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -866,7 +866,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>